<commit_message>
.html actualizacion  y creacion de style.css
</commit_message>
<xml_diff>
--- a/resultados/resultado_diabetes.xlsx
+++ b/resultados/resultado_diabetes.xlsx
@@ -482,28 +482,28 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>

</xml_diff>